<commit_message>
add workflow rerun results
</commit_message>
<xml_diff>
--- a/results/tables/hub_genes.xlsx
+++ b/results/tables/hub_genes.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t xml:space="preserve">module</t>
   </si>
@@ -256,31 +248,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -292,7 +268,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -300,382 +276,614 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14">
+      <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15">
+      <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18">
+      <c r="A18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20">
+      <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21">
+      <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22">
+      <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23">
+      <c r="A23" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24">
+      <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25">
+      <c r="A25" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26">
+      <c r="A26" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27">
+      <c r="A27" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28">
+      <c r="A28" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>